<commit_message>
fixed login bug and deleted docs
</commit_message>
<xml_diff>
--- a/Administratie/Logboeken/DaanLogboek.xlsx
+++ b/Administratie/Logboeken/DaanLogboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a575cd3af734844/Bureaublad/Proccess and tools/Proccess-and-tools/Administratie/Logboeken/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8_{4FB24395-E28A-4155-BC7C-245B3C5CD175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8_{180D0A6E-270C-4FB9-AE2B-039F0FAB7341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="14" uniqueCount="14">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="15" uniqueCount="15">
   <si>
     <t>datum</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>comments bij de code plaatsen</t>
+  </si>
+  <si>
+    <t>comments bij de code plaatsen in de main.py</t>
   </si>
 </sst>
 </file>
@@ -435,8 +438,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +536,15 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="d">
+        <v>2024-09-14</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>